<commit_message>
Arreglada fecha y añadido nuevos parámetros
</commit_message>
<xml_diff>
--- a/cotizaciones.xlsx
+++ b/cotizaciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\OneDrive\Escritorio\Claudia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Proyectos\Personales\Python Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4B7385-988D-44EA-8D00-5A1CB4F9FA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403B8E4A-C17A-454E-951B-838AAD746004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{57AC7185-5362-4E71-917C-5F60B0BBA445}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="198">
   <si>
     <t>origen</t>
   </si>
@@ -672,9 +672,6 @@
   </si>
   <si>
     <t>precio total cot</t>
-  </si>
-  <si>
-    <t>sfjlksdjflskdjfsdlkfjsdlkfjsdlkfjsklfjdslkfjsdlkfjsd</t>
   </si>
 </sst>
 </file>
@@ -1422,12 +1419,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{259CBBF0-11C7-4E6E-BCAD-DB8B09504BE8}">
-  <dimension ref="A1:W66"/>
+  <dimension ref="A1:W65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -1546,7 +1543,7 @@
         <v>53</v>
       </c>
       <c r="J2" s="19">
-        <f t="shared" ref="J2:J54" si="0">N2*P2*Q2*R2</f>
+        <f t="shared" ref="J2:J53" si="0">N2*P2*Q2*R2</f>
         <v>377.48591999999996</v>
       </c>
       <c r="K2" s="19">
@@ -1617,7 +1614,7 @@
         <v>777.93371999999999</v>
       </c>
       <c r="K3" s="19">
-        <f t="shared" ref="K3:K56" si="1">J3*H3</f>
+        <f t="shared" ref="K3:K55" si="1">J3*H3</f>
         <v>3111.73488</v>
       </c>
       <c r="L3" s="4" t="s">
@@ -1961,13 +1958,13 @@
       <c r="I9" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="J9" s="19">
-        <f>(N10+N9)*P9*Q9*R9</f>
-        <v>14587.5141</v>
-      </c>
-      <c r="K9" s="19">
+      <c r="J9" s="19" t="e">
+        <f>(#REF!+N9)*P9*Q9*R9</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K9" s="19" t="e">
         <f t="shared" si="1"/>
-        <v>29175.028200000001</v>
+        <v>#REF!</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>84</v>
@@ -2003,48 +2000,75 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10">
-        <v>3</v>
-      </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10">
-        <v>0</v>
-      </c>
-      <c r="H10" s="11">
-        <v>1</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="J10" s="34">
+    <row r="10" spans="1:23" ht="24" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>45349</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="4">
+        <v>4</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5">
+        <v>1</v>
+      </c>
+      <c r="I10" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="J10" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>222.03800000000001</v>
       </c>
       <c r="K10" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10">
-        <v>1851990</v>
-      </c>
-      <c r="N10" s="34">
-        <v>1532.55</v>
-      </c>
-      <c r="O10" s="13"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
+        <v>222.03800000000001</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="M10" s="4">
+        <v>56584</v>
+      </c>
+      <c r="N10" s="19">
+        <v>82.85</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P10" s="6">
+        <v>2.68</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>1</v>
+      </c>
+      <c r="R10" s="6">
+        <v>1</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="V10" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:23" ht="24" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -2066,30 +2090,27 @@
         <v>90</v>
       </c>
       <c r="G11" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11" s="5">
         <v>1</v>
       </c>
       <c r="I11" s="49" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J11" s="19">
         <f t="shared" si="0"/>
-        <v>222.03800000000001</v>
+        <v>116.12440000000001</v>
       </c>
       <c r="K11" s="19">
         <f t="shared" si="1"/>
-        <v>222.03800000000001</v>
+        <v>116.12440000000001</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="M11" s="4">
-        <v>56584</v>
+        <v>96</v>
       </c>
       <c r="N11" s="19">
-        <v>82.85</v>
+        <v>43.33</v>
       </c>
       <c r="O11" s="7" t="s">
         <v>1</v>
@@ -2103,20 +2124,8 @@
       <c r="R11" s="6">
         <v>1</v>
       </c>
-      <c r="S11" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="U11" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="V11" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" ht="24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>45349</v>
       </c>
@@ -2136,27 +2145,27 @@
         <v>90</v>
       </c>
       <c r="G12" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H12" s="5">
         <v>1</v>
       </c>
       <c r="I12" s="49" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="J12" s="19">
         <f t="shared" si="0"/>
-        <v>116.12440000000001</v>
+        <v>7619.3472000000011</v>
       </c>
       <c r="K12" s="19">
         <f t="shared" si="1"/>
-        <v>116.12440000000001</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>96</v>
+        <v>7619.3472000000011</v>
+      </c>
+      <c r="M12" s="33">
+        <v>5300600</v>
       </c>
       <c r="N12" s="19">
-        <v>43.33</v>
+        <v>5923</v>
       </c>
       <c r="O12" s="7" t="s">
         <v>1</v>
@@ -2165,10 +2174,22 @@
         <v>2.68</v>
       </c>
       <c r="Q12" s="6">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="R12" s="6">
-        <v>1</v>
+        <v>0.8</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="U12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="V12" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
@@ -2191,30 +2212,27 @@
         <v>90</v>
       </c>
       <c r="G13" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H13" s="5">
         <v>1</v>
       </c>
       <c r="I13" s="49" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J13" s="19">
         <f t="shared" si="0"/>
-        <v>7619.3472000000011</v>
+        <v>106.51391999999998</v>
       </c>
       <c r="K13" s="19">
         <f t="shared" si="1"/>
-        <v>7619.3472000000011</v>
+        <v>106.51391999999998</v>
       </c>
       <c r="M13" s="33">
-        <v>5300600</v>
+        <v>5300602</v>
       </c>
       <c r="N13" s="19">
-        <v>5923</v>
-      </c>
-      <c r="O13" s="7" t="s">
-        <v>1</v>
+        <v>82.8</v>
       </c>
       <c r="P13" s="6">
         <v>2.68</v>
@@ -2224,18 +2242,6 @@
       </c>
       <c r="R13" s="6">
         <v>0.8</v>
-      </c>
-      <c r="S13" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="T13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="U13" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="V13" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -2258,27 +2264,27 @@
         <v>90</v>
       </c>
       <c r="G14" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H14" s="5">
         <v>1</v>
       </c>
       <c r="I14" s="49" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J14" s="19">
         <f t="shared" si="0"/>
-        <v>106.51391999999998</v>
+        <v>311.56608000000006</v>
       </c>
       <c r="K14" s="19">
         <f t="shared" si="1"/>
-        <v>106.51391999999998</v>
-      </c>
-      <c r="M14" s="33">
-        <v>5300602</v>
+        <v>311.56608000000006</v>
+      </c>
+      <c r="M14" s="4">
+        <v>5300603</v>
       </c>
       <c r="N14" s="19">
-        <v>82.8</v>
+        <v>242.2</v>
       </c>
       <c r="P14" s="6">
         <v>2.68</v>
@@ -2310,27 +2316,27 @@
         <v>90</v>
       </c>
       <c r="G15" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H15" s="5">
         <v>1</v>
       </c>
       <c r="I15" s="49" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J15" s="19">
         <f t="shared" si="0"/>
-        <v>311.56608000000006</v>
+        <v>1161.2332800000001</v>
       </c>
       <c r="K15" s="19">
         <f t="shared" si="1"/>
-        <v>311.56608000000006</v>
+        <v>1161.2332800000001</v>
       </c>
       <c r="M15" s="4">
-        <v>5300603</v>
+        <v>5300604</v>
       </c>
       <c r="N15" s="19">
-        <v>242.2</v>
+        <v>902.7</v>
       </c>
       <c r="P15" s="6">
         <v>2.68</v>
@@ -2362,27 +2368,27 @@
         <v>90</v>
       </c>
       <c r="G16" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H16" s="5">
         <v>1</v>
       </c>
       <c r="I16" s="49" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J16" s="19">
         <f t="shared" si="0"/>
-        <v>1161.2332800000001</v>
+        <v>1408.0934399999999</v>
       </c>
       <c r="K16" s="19">
         <f t="shared" si="1"/>
-        <v>1161.2332800000001</v>
+        <v>1408.0934399999999</v>
       </c>
       <c r="M16" s="4">
-        <v>5300604</v>
+        <v>5300605</v>
       </c>
       <c r="N16" s="19">
-        <v>902.7</v>
+        <v>1094.5999999999999</v>
       </c>
       <c r="P16" s="6">
         <v>2.68</v>
@@ -2414,27 +2420,27 @@
         <v>90</v>
       </c>
       <c r="G17" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H17" s="5">
         <v>1</v>
       </c>
       <c r="I17" s="49" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J17" s="19">
         <f t="shared" si="0"/>
-        <v>1408.0934399999999</v>
+        <v>1199.9539199999999</v>
       </c>
       <c r="K17" s="19">
         <f t="shared" si="1"/>
-        <v>1408.0934399999999</v>
+        <v>1199.9539199999999</v>
       </c>
       <c r="M17" s="4">
-        <v>5300605</v>
+        <v>5300606</v>
       </c>
       <c r="N17" s="19">
-        <v>1094.5999999999999</v>
+        <v>932.8</v>
       </c>
       <c r="P17" s="6">
         <v>2.68</v>
@@ -2466,27 +2472,27 @@
         <v>90</v>
       </c>
       <c r="G18" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H18" s="5">
         <v>1</v>
       </c>
       <c r="I18" s="49" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J18" s="19">
         <f t="shared" si="0"/>
-        <v>1199.9539199999999</v>
+        <v>925.82208000000014</v>
       </c>
       <c r="K18" s="19">
         <f t="shared" si="1"/>
-        <v>1199.9539199999999</v>
+        <v>925.82208000000014</v>
       </c>
       <c r="M18" s="4">
-        <v>5300606</v>
+        <v>5300607</v>
       </c>
       <c r="N18" s="19">
-        <v>932.8</v>
+        <v>719.7</v>
       </c>
       <c r="P18" s="6">
         <v>2.68</v>
@@ -2498,7 +2504,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>45349</v>
       </c>
@@ -2518,39 +2524,48 @@
         <v>90</v>
       </c>
       <c r="G19" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H19" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I19" s="49" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J19" s="19">
         <f t="shared" si="0"/>
-        <v>925.82208000000014</v>
+        <v>270.68</v>
       </c>
       <c r="K19" s="19">
         <f t="shared" si="1"/>
-        <v>925.82208000000014</v>
+        <v>812.04</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="M19" s="4">
-        <v>5300607</v>
+        <v>5281328</v>
       </c>
       <c r="N19" s="19">
-        <v>719.7</v>
+        <v>202</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>1</v>
       </c>
       <c r="P19" s="6">
         <v>2.68</v>
       </c>
       <c r="Q19" s="6">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="R19" s="6">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="V19" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="60.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>45349</v>
       </c>
@@ -2569,113 +2584,122 @@
       <c r="F20" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G20" s="4">
-        <v>10</v>
-      </c>
-      <c r="H20" s="5">
-        <v>3</v>
-      </c>
-      <c r="I20" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="J20" s="19">
+      <c r="G20" s="35">
+        <v>11</v>
+      </c>
+      <c r="H20" s="36">
+        <v>2</v>
+      </c>
+      <c r="I20" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="J20" s="39">
         <f t="shared" si="0"/>
-        <v>270.68</v>
+        <v>7251.9</v>
       </c>
       <c r="K20" s="19">
         <f t="shared" si="1"/>
-        <v>812.04</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="M20" s="4">
-        <v>5281328</v>
-      </c>
-      <c r="N20" s="19">
-        <v>202</v>
-      </c>
-      <c r="O20" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="P20" s="6">
-        <v>2.68</v>
-      </c>
-      <c r="Q20" s="6">
+        <v>14503.8</v>
+      </c>
+      <c r="L20" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="M20" s="35">
+        <v>5282302</v>
+      </c>
+      <c r="N20" s="39">
+        <v>6306</v>
+      </c>
+      <c r="O20" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="P20" s="38">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Q20" s="38">
         <v>0.5</v>
       </c>
-      <c r="R20" s="6">
-        <v>1</v>
-      </c>
-      <c r="V20" s="4" t="s">
+      <c r="R20" s="38">
+        <v>1</v>
+      </c>
+      <c r="S20" s="35"/>
+      <c r="T20" s="35"/>
+      <c r="U20" s="35"/>
+      <c r="V20" s="35" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="60.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>45349</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="D21" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G21" s="35">
-        <v>11</v>
-      </c>
-      <c r="H21" s="36">
-        <v>2</v>
-      </c>
-      <c r="I21" s="50" t="s">
-        <v>105</v>
-      </c>
-      <c r="J21" s="39">
+        <v>110</v>
+      </c>
+      <c r="G21" s="4">
+        <v>1</v>
+      </c>
+      <c r="H21" s="5">
+        <v>6</v>
+      </c>
+      <c r="I21" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="J21" s="19">
         <f t="shared" si="0"/>
-        <v>7251.9</v>
+        <v>893.13299999999992</v>
       </c>
       <c r="K21" s="19">
         <f t="shared" si="1"/>
-        <v>14503.8</v>
-      </c>
-      <c r="L21" s="35" t="s">
-        <v>107</v>
-      </c>
-      <c r="M21" s="35">
-        <v>5282302</v>
-      </c>
-      <c r="N21" s="39">
-        <v>6306</v>
-      </c>
-      <c r="O21" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="P21" s="38">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="Q21" s="38">
-        <v>0.5</v>
-      </c>
-      <c r="R21" s="38">
-        <v>1</v>
-      </c>
-      <c r="S21" s="35"/>
-      <c r="T21" s="35"/>
-      <c r="U21" s="35"/>
-      <c r="V21" s="35" t="s">
+        <v>5358.7979999999998</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M21" s="4">
+        <v>1841451</v>
+      </c>
+      <c r="N21" s="19">
+        <v>261.14999999999998</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P21" s="6">
+        <v>3.42</v>
+      </c>
+      <c r="Q21" s="6">
+        <v>1</v>
+      </c>
+      <c r="R21" s="6">
+        <v>1</v>
+      </c>
+      <c r="S21" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="T21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="U21" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="V21" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" ht="84" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>45349</v>
       </c>
@@ -2694,192 +2718,192 @@
       <c r="F22" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="G22" s="4">
-        <v>1</v>
-      </c>
-      <c r="H22" s="5">
-        <v>6</v>
-      </c>
-      <c r="I22" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="J22" s="19">
+      <c r="G22" s="10">
+        <v>2</v>
+      </c>
+      <c r="H22" s="11">
+        <v>5</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="J22" s="34">
         <f t="shared" si="0"/>
-        <v>893.13299999999992</v>
+        <v>1076.69</v>
       </c>
       <c r="K22" s="19">
         <f t="shared" si="1"/>
-        <v>5358.7979999999998</v>
-      </c>
-      <c r="L22" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="M22" s="4">
-        <v>1841451</v>
-      </c>
-      <c r="N22" s="19">
-        <v>261.14999999999998</v>
-      </c>
-      <c r="O22" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="P22" s="6">
-        <v>3.42</v>
-      </c>
-      <c r="Q22" s="6">
-        <v>1</v>
-      </c>
-      <c r="R22" s="6">
-        <v>1</v>
-      </c>
-      <c r="S22" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="T22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="U22" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="V22" s="4" t="s">
+        <v>5383.4500000000007</v>
+      </c>
+      <c r="L22" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="M22" s="10">
+        <v>457390</v>
+      </c>
+      <c r="N22" s="34">
+        <v>803.5</v>
+      </c>
+      <c r="O22" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="P22" s="12">
+        <v>2.68</v>
+      </c>
+      <c r="Q22" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="R22" s="12">
+        <v>1</v>
+      </c>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="84" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>45349</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D23" s="4">
-        <v>5</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G23" s="10">
-        <v>2</v>
-      </c>
-      <c r="H23" s="11">
-        <v>5</v>
-      </c>
-      <c r="I23" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="J23" s="34">
+    <row r="23" spans="1:23" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="43">
+        <v>45350</v>
+      </c>
+      <c r="B23" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23" s="44">
+        <v>6</v>
+      </c>
+      <c r="E23" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" s="44">
+        <v>1</v>
+      </c>
+      <c r="H23" s="45">
+        <v>1</v>
+      </c>
+      <c r="I23" s="51" t="s">
+        <v>117</v>
+      </c>
+      <c r="J23" s="47">
         <f t="shared" si="0"/>
-        <v>1076.69</v>
+        <v>1208.2378000000001</v>
       </c>
       <c r="K23" s="19">
         <f t="shared" si="1"/>
-        <v>5383.4500000000007</v>
-      </c>
-      <c r="L23" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="M23" s="10">
-        <v>457390</v>
-      </c>
-      <c r="N23" s="34">
-        <v>803.5</v>
-      </c>
-      <c r="O23" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="P23" s="12">
+        <v>1208.2378000000001</v>
+      </c>
+      <c r="L23" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="M23" s="44">
+        <v>459490</v>
+      </c>
+      <c r="N23" s="47">
+        <v>901.67</v>
+      </c>
+      <c r="O23" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="P23" s="46">
         <v>2.68</v>
       </c>
-      <c r="Q23" s="12">
+      <c r="Q23" s="46">
         <v>0.5</v>
       </c>
-      <c r="R23" s="12">
-        <v>1</v>
-      </c>
-      <c r="S23" s="10"/>
-      <c r="T23" s="10"/>
-      <c r="U23" s="10"/>
-      <c r="V23" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="43">
+      <c r="R23" s="46">
+        <v>1</v>
+      </c>
+      <c r="S23" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="T23" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="U23" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="V23" s="44" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" s="8" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="52">
         <v>45350</v>
       </c>
-      <c r="B24" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="C24" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="D24" s="44">
-        <v>6</v>
-      </c>
-      <c r="E24" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="G24" s="44">
-        <v>1</v>
-      </c>
-      <c r="H24" s="45">
-        <v>1</v>
-      </c>
-      <c r="I24" s="51" t="s">
-        <v>117</v>
-      </c>
-      <c r="J24" s="47">
+      <c r="B24" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D24" s="8">
+        <v>7</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="G24" s="8">
+        <v>1</v>
+      </c>
+      <c r="H24" s="53">
+        <v>2</v>
+      </c>
+      <c r="I24" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="J24" s="55">
         <f t="shared" si="0"/>
-        <v>1208.2378000000001</v>
+        <v>476.65140000000002</v>
       </c>
       <c r="K24" s="19">
         <f t="shared" si="1"/>
-        <v>1208.2378000000001</v>
-      </c>
-      <c r="L24" s="44" t="s">
-        <v>121</v>
-      </c>
-      <c r="M24" s="44">
-        <v>459490</v>
-      </c>
-      <c r="N24" s="47">
-        <v>901.67</v>
-      </c>
-      <c r="O24" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="P24" s="46">
+        <v>953.30280000000005</v>
+      </c>
+      <c r="L24" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="M24" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="N24" s="55">
+        <v>355.71</v>
+      </c>
+      <c r="O24" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="P24" s="54">
         <v>2.68</v>
       </c>
-      <c r="Q24" s="46">
+      <c r="Q24" s="54">
         <v>0.5</v>
       </c>
-      <c r="R24" s="46">
-        <v>1</v>
-      </c>
-      <c r="S24" s="44" t="s">
+      <c r="R24" s="54">
+        <v>1</v>
+      </c>
+      <c r="S24" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="T24" s="44" t="s">
+      <c r="T24" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="U24" s="44" t="s">
+      <c r="U24" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="V24" s="44" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" s="8" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V24" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" s="8" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="52">
         <v>45350</v>
       </c>
@@ -2899,30 +2923,30 @@
         <v>136</v>
       </c>
       <c r="G25" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H25" s="53">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I25" s="49" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J25" s="55">
         <f t="shared" si="0"/>
-        <v>476.65140000000002</v>
+        <v>245.89000000000001</v>
       </c>
       <c r="K25" s="19">
         <f t="shared" si="1"/>
-        <v>953.30280000000005</v>
+        <v>983.56000000000006</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N25" s="55">
-        <v>355.71</v>
+        <v>183.5</v>
       </c>
       <c r="O25" s="49" t="s">
         <v>1</v>
@@ -2936,20 +2960,11 @@
       <c r="R25" s="54">
         <v>1</v>
       </c>
-      <c r="S25" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="T25" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="U25" s="8" t="s">
-        <v>77</v>
-      </c>
       <c r="V25" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:23" s="8" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" s="8" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="52">
         <v>45350</v>
       </c>
@@ -2969,30 +2984,30 @@
         <v>136</v>
       </c>
       <c r="G26" s="8">
+        <v>3</v>
+      </c>
+      <c r="H26" s="53">
         <v>2</v>
       </c>
-      <c r="H26" s="53">
-        <v>4</v>
-      </c>
       <c r="I26" s="49" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J26" s="55">
         <f t="shared" si="0"/>
-        <v>245.89000000000001</v>
+        <v>552.08000000000004</v>
       </c>
       <c r="K26" s="19">
         <f t="shared" si="1"/>
-        <v>983.56000000000006</v>
+        <v>1104.1600000000001</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="M26" s="8" t="s">
-        <v>133</v>
+        <v>129</v>
+      </c>
+      <c r="M26" s="8">
+        <v>50932</v>
       </c>
       <c r="N26" s="55">
-        <v>183.5</v>
+        <v>412</v>
       </c>
       <c r="O26" s="49" t="s">
         <v>1</v>
@@ -3007,7 +3022,7 @@
         <v>1</v>
       </c>
       <c r="V26" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:23" s="8" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -3030,30 +3045,30 @@
         <v>136</v>
       </c>
       <c r="G27" s="8">
+        <v>4</v>
+      </c>
+      <c r="H27" s="53">
         <v>3</v>
       </c>
-      <c r="H27" s="53">
-        <v>2</v>
-      </c>
       <c r="I27" s="49" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J27" s="55">
         <f t="shared" si="0"/>
-        <v>552.08000000000004</v>
+        <v>600.65500000000009</v>
       </c>
       <c r="K27" s="19">
         <f t="shared" si="1"/>
-        <v>1104.1600000000001</v>
+        <v>1801.9650000000001</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="M27" s="8">
-        <v>50932</v>
+        <v>50933</v>
       </c>
       <c r="N27" s="55">
-        <v>412</v>
+        <v>448.25</v>
       </c>
       <c r="O27" s="49" t="s">
         <v>1</v>
@@ -3071,7 +3086,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:23" s="8" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" s="8" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="52">
         <v>45350</v>
       </c>
@@ -3090,113 +3105,122 @@
       <c r="F28" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="G28" s="8">
-        <v>4</v>
-      </c>
-      <c r="H28" s="53">
-        <v>3</v>
-      </c>
-      <c r="I28" s="49" t="s">
-        <v>125</v>
-      </c>
-      <c r="J28" s="55">
+      <c r="G28" s="37">
+        <v>5</v>
+      </c>
+      <c r="H28" s="56">
+        <v>1</v>
+      </c>
+      <c r="I28" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="J28" s="58">
         <f t="shared" si="0"/>
-        <v>600.65500000000009</v>
-      </c>
-      <c r="K28" s="19">
+        <v>76.688199999999995</v>
+      </c>
+      <c r="K28" s="34">
         <f t="shared" si="1"/>
-        <v>1801.9650000000001</v>
-      </c>
-      <c r="L28" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="M28" s="8">
-        <v>50933</v>
-      </c>
-      <c r="N28" s="55">
-        <v>448.25</v>
-      </c>
-      <c r="O28" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="P28" s="54">
+        <v>76.688199999999995</v>
+      </c>
+      <c r="L28" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="M28" s="37">
+        <v>60311</v>
+      </c>
+      <c r="N28" s="58">
+        <v>57.23</v>
+      </c>
+      <c r="O28" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="P28" s="57">
         <v>2.68</v>
       </c>
-      <c r="Q28" s="54">
+      <c r="Q28" s="57">
         <v>0.5</v>
       </c>
-      <c r="R28" s="54">
-        <v>1</v>
-      </c>
-      <c r="V28" s="8" t="s">
+      <c r="R28" s="57">
+        <v>1</v>
+      </c>
+      <c r="S28" s="37"/>
+      <c r="T28" s="37"/>
+      <c r="U28" s="37"/>
+      <c r="V28" s="37" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:23" s="8" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" s="8" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="52">
         <v>45350</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="D29" s="8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="G29" s="37">
-        <v>5</v>
-      </c>
-      <c r="H29" s="56">
-        <v>1</v>
-      </c>
-      <c r="I29" s="50" t="s">
-        <v>126</v>
-      </c>
-      <c r="J29" s="58">
+        <v>146</v>
+      </c>
+      <c r="G29" s="8">
+        <v>1</v>
+      </c>
+      <c r="H29" s="53">
+        <v>3</v>
+      </c>
+      <c r="I29" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="J29" s="55">
         <f t="shared" si="0"/>
-        <v>76.688199999999995</v>
-      </c>
-      <c r="K29" s="34">
+        <v>476.65140000000002</v>
+      </c>
+      <c r="K29" s="19">
         <f t="shared" si="1"/>
-        <v>76.688199999999995</v>
-      </c>
-      <c r="L29" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="M29" s="37">
-        <v>60311</v>
-      </c>
-      <c r="N29" s="58">
-        <v>57.23</v>
-      </c>
-      <c r="O29" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="P29" s="57">
+        <v>1429.9542000000001</v>
+      </c>
+      <c r="L29" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="M29" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="N29" s="55">
+        <v>355.71</v>
+      </c>
+      <c r="O29" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="P29" s="54">
         <v>2.68</v>
       </c>
-      <c r="Q29" s="57">
+      <c r="Q29" s="54">
         <v>0.5</v>
       </c>
-      <c r="R29" s="57">
-        <v>1</v>
-      </c>
-      <c r="S29" s="37"/>
-      <c r="T29" s="37"/>
-      <c r="U29" s="37"/>
-      <c r="V29" s="37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" s="8" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R29" s="54">
+        <v>1</v>
+      </c>
+      <c r="S29" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="T29" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="U29" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="V29" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" s="8" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="52">
         <v>45350</v>
       </c>
@@ -3216,30 +3240,30 @@
         <v>146</v>
       </c>
       <c r="G30" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H30" s="53">
         <v>3</v>
       </c>
       <c r="I30" s="49" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="J30" s="55">
         <f t="shared" si="0"/>
-        <v>476.65140000000002</v>
+        <v>305.13140000000004</v>
       </c>
       <c r="K30" s="19">
         <f t="shared" si="1"/>
-        <v>1429.9542000000001</v>
+        <v>915.39420000000018</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="M30" s="8" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="N30" s="55">
-        <v>355.71</v>
+        <v>227.71</v>
       </c>
       <c r="O30" s="49" t="s">
         <v>1</v>
@@ -3253,20 +3277,11 @@
       <c r="R30" s="54">
         <v>1</v>
       </c>
-      <c r="S30" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="T30" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="U30" s="8" t="s">
-        <v>77</v>
-      </c>
       <c r="V30" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" s="8" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="52">
         <v>45350</v>
       </c>
@@ -3285,116 +3300,125 @@
       <c r="F31" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="G31" s="8">
-        <v>2</v>
-      </c>
-      <c r="H31" s="53">
+      <c r="G31" s="35">
         <v>3</v>
       </c>
-      <c r="I31" s="49" t="s">
-        <v>137</v>
-      </c>
-      <c r="J31" s="55">
-        <f t="shared" si="0"/>
-        <v>305.13140000000004</v>
-      </c>
-      <c r="K31" s="19">
-        <f t="shared" si="1"/>
-        <v>915.39420000000018</v>
-      </c>
-      <c r="L31" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="M31" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="N31" s="55">
-        <v>227.71</v>
-      </c>
-      <c r="O31" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="P31" s="54">
-        <v>2.68</v>
-      </c>
-      <c r="Q31" s="54">
-        <v>0.5</v>
-      </c>
-      <c r="R31" s="54">
-        <v>1</v>
-      </c>
-      <c r="V31" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="52">
-        <v>45350</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="D32" s="8">
-        <v>8</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="G32" s="35">
+      <c r="H31" s="36">
         <v>3</v>
       </c>
-      <c r="H32" s="36">
-        <v>3</v>
-      </c>
-      <c r="I32" s="50" t="s">
+      <c r="I31" s="50" t="s">
         <v>140</v>
       </c>
-      <c r="J32" s="39">
+      <c r="J31" s="39">
         <f t="shared" si="0"/>
         <v>640.09120000000007</v>
       </c>
-      <c r="K32" s="39">
+      <c r="K31" s="39">
         <f t="shared" si="1"/>
         <v>1920.2736000000002</v>
       </c>
-      <c r="L32" s="35" t="s">
+      <c r="L31" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="M32" s="35">
+      <c r="M31" s="35">
         <v>62762</v>
       </c>
-      <c r="N32" s="39">
+      <c r="N31" s="39">
         <v>477.68</v>
       </c>
-      <c r="O32" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="P32" s="38">
+      <c r="O31" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="P31" s="38">
         <v>2.68</v>
       </c>
-      <c r="Q32" s="38">
+      <c r="Q31" s="38">
         <v>0.5</v>
       </c>
-      <c r="R32" s="38">
-        <v>1</v>
-      </c>
-      <c r="S32" s="35"/>
-      <c r="T32" s="35"/>
-      <c r="U32" s="35"/>
+      <c r="R31" s="38">
+        <v>1</v>
+      </c>
+      <c r="S31" s="35"/>
+      <c r="T31" s="35"/>
+      <c r="U31" s="35"/>
+      <c r="V31" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="W31" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>45351</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D32" s="4">
+        <v>9</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G32" s="4">
+        <v>1</v>
+      </c>
+      <c r="H32" s="5">
+        <v>26</v>
+      </c>
+      <c r="I32" s="49" t="s">
+        <v>151</v>
+      </c>
+      <c r="J32" s="19">
+        <f t="shared" si="0"/>
+        <v>231.09640000000002</v>
+      </c>
+      <c r="K32" s="19">
+        <f t="shared" si="1"/>
+        <v>6008.5064000000002</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="M32" s="59">
+        <v>528747</v>
+      </c>
+      <c r="N32" s="19">
+        <v>172.46</v>
+      </c>
+      <c r="O32" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P32" s="6">
+        <v>2.68</v>
+      </c>
+      <c r="Q32" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R32" s="6">
+        <v>1</v>
+      </c>
+      <c r="S32" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="T32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="U32" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="V32" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="W32" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>45351</v>
       </c>
@@ -3414,30 +3438,30 @@
         <v>156</v>
       </c>
       <c r="G33" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H33" s="5">
         <v>26</v>
       </c>
       <c r="I33" s="49" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="J33" s="19">
         <f t="shared" si="0"/>
-        <v>231.09640000000002</v>
+        <v>535.12900000000002</v>
       </c>
       <c r="K33" s="19">
         <f t="shared" si="1"/>
-        <v>6008.5064000000002</v>
+        <v>13913.354000000001</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="M33" s="59">
-        <v>528747</v>
+        <v>129</v>
+      </c>
+      <c r="M33" s="4">
+        <v>66667</v>
       </c>
       <c r="N33" s="19">
-        <v>172.46</v>
+        <v>399.35</v>
       </c>
       <c r="O33" s="7" t="s">
         <v>1</v>
@@ -3451,20 +3475,11 @@
       <c r="R33" s="6">
         <v>1</v>
       </c>
-      <c r="S33" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="T33" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="U33" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="V33" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" ht="72" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>45351</v>
       </c>
@@ -3484,30 +3499,30 @@
         <v>156</v>
       </c>
       <c r="G34" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H34" s="5">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="I34" s="49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J34" s="19">
         <f t="shared" si="0"/>
-        <v>535.12900000000002</v>
+        <v>4315.6147200000005</v>
       </c>
       <c r="K34" s="19">
         <f t="shared" si="1"/>
-        <v>13913.354000000001</v>
+        <v>43156.147200000007</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="M34" s="4">
-        <v>66667</v>
+        <v>173</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="N34" s="19">
-        <v>399.35</v>
+        <v>2683.84</v>
       </c>
       <c r="O34" s="7" t="s">
         <v>1</v>
@@ -3516,7 +3531,7 @@
         <v>2.68</v>
       </c>
       <c r="Q34" s="6">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="R34" s="6">
         <v>1</v>
@@ -3525,7 +3540,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="72" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" ht="48.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>45351</v>
       </c>
@@ -3544,110 +3559,119 @@
       <c r="F35" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="G35" s="4">
-        <v>3</v>
-      </c>
-      <c r="H35" s="5">
-        <v>10</v>
-      </c>
-      <c r="I35" s="49" t="s">
-        <v>171</v>
-      </c>
-      <c r="J35" s="19">
+      <c r="G35" s="35">
+        <v>4</v>
+      </c>
+      <c r="H35" s="36">
+        <v>14</v>
+      </c>
+      <c r="I35" s="50" t="s">
+        <v>152</v>
+      </c>
+      <c r="J35" s="39">
         <f t="shared" si="0"/>
-        <v>4315.6147200000005</v>
-      </c>
-      <c r="K35" s="19">
+        <v>1715.6154000000001</v>
+      </c>
+      <c r="K35" s="39">
         <f t="shared" si="1"/>
-        <v>43156.147200000007</v>
-      </c>
-      <c r="L35" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="M35" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="N35" s="19">
-        <v>2683.84</v>
-      </c>
-      <c r="O35" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="P35" s="6">
+        <v>24018.615600000001</v>
+      </c>
+      <c r="L35" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="M35" s="35">
+        <v>232790</v>
+      </c>
+      <c r="N35" s="39">
+        <v>1280.31</v>
+      </c>
+      <c r="O35" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="P35" s="38">
         <v>2.68</v>
       </c>
-      <c r="Q35" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="R35" s="6">
-        <v>1</v>
-      </c>
-      <c r="V35" s="4" t="s">
+      <c r="Q35" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="R35" s="38">
+        <v>1</v>
+      </c>
+      <c r="S35" s="35"/>
+      <c r="T35" s="35"/>
+      <c r="U35" s="35"/>
+      <c r="V35" s="35" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="48.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" ht="48" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>45351</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D36" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>28</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="G36" s="35">
-        <v>4</v>
-      </c>
-      <c r="H36" s="36">
-        <v>14</v>
-      </c>
-      <c r="I36" s="50" t="s">
-        <v>152</v>
-      </c>
-      <c r="J36" s="39">
-        <f t="shared" si="0"/>
-        <v>1715.6154000000001</v>
-      </c>
-      <c r="K36" s="39">
-        <f t="shared" si="1"/>
-        <v>24018.615600000001</v>
-      </c>
-      <c r="L36" s="35" t="s">
-        <v>154</v>
-      </c>
-      <c r="M36" s="35">
-        <v>232790</v>
-      </c>
-      <c r="N36" s="39">
-        <v>1280.31</v>
-      </c>
-      <c r="O36" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="P36" s="38">
+        <v>159</v>
+      </c>
+      <c r="G36" s="8">
+        <v>1</v>
+      </c>
+      <c r="H36" s="53">
+        <v>3</v>
+      </c>
+      <c r="I36" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="J36" s="55">
+        <f t="shared" ref="J36:J38" si="2">N36*P36*Q36*R36</f>
+        <v>476.65140000000002</v>
+      </c>
+      <c r="K36" s="19">
+        <f t="shared" ref="K36:K38" si="3">J36*H36</f>
+        <v>1429.9542000000001</v>
+      </c>
+      <c r="L36" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="M36" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="N36" s="55">
+        <v>355.71</v>
+      </c>
+      <c r="O36" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P36" s="6">
         <v>2.68</v>
       </c>
-      <c r="Q36" s="38">
+      <c r="Q36" s="6">
         <v>0.5</v>
       </c>
-      <c r="R36" s="38">
-        <v>1</v>
-      </c>
-      <c r="S36" s="35"/>
-      <c r="T36" s="35"/>
-      <c r="U36" s="35"/>
-      <c r="V36" s="35" t="s">
-        <v>14</v>
+      <c r="R36" s="6">
+        <v>1</v>
+      </c>
+      <c r="S36" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="T36" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="U36" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="V36" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:23" ht="48" x14ac:dyDescent="0.25">
@@ -3670,30 +3694,30 @@
         <v>159</v>
       </c>
       <c r="G37" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H37" s="53">
         <v>3</v>
       </c>
       <c r="I37" s="49" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="J37" s="55">
-        <f t="shared" ref="J37:J39" si="2">N37*P37*Q37*R37</f>
-        <v>476.65140000000002</v>
+        <f t="shared" si="2"/>
+        <v>305.13140000000004</v>
       </c>
       <c r="K37" s="19">
-        <f t="shared" ref="K37:K39" si="3">J37*H37</f>
-        <v>1429.9542000000001</v>
+        <f t="shared" si="3"/>
+        <v>915.39420000000018</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="M37" s="8" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="N37" s="55">
-        <v>355.71</v>
+        <v>227.71</v>
       </c>
       <c r="O37" s="7" t="s">
         <v>1</v>
@@ -3707,20 +3731,11 @@
       <c r="R37" s="6">
         <v>1</v>
       </c>
-      <c r="S37" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="T37" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="U37" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="V37" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:23" ht="48" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" ht="60.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>45351</v>
       </c>
@@ -3739,112 +3754,118 @@
       <c r="F38" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="G38" s="8">
-        <v>2</v>
-      </c>
-      <c r="H38" s="53">
+      <c r="G38" s="35">
         <v>3</v>
       </c>
-      <c r="I38" s="49" t="s">
-        <v>137</v>
-      </c>
-      <c r="J38" s="55">
-        <f t="shared" si="2"/>
-        <v>305.13140000000004</v>
-      </c>
-      <c r="K38" s="19">
-        <f t="shared" si="3"/>
-        <v>915.39420000000018</v>
-      </c>
-      <c r="L38" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="M38" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="N38" s="55">
-        <v>227.71</v>
-      </c>
-      <c r="O38" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="P38" s="6">
-        <v>2.68</v>
-      </c>
-      <c r="Q38" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="R38" s="6">
-        <v>1</v>
-      </c>
-      <c r="V38" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23" ht="60.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="3">
-        <v>45351</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="D39" s="4">
-        <v>10</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="G39" s="35">
+      <c r="H38" s="36">
         <v>3</v>
       </c>
-      <c r="H39" s="36">
-        <v>3</v>
-      </c>
-      <c r="I39" s="50" t="s">
+      <c r="I38" s="50" t="s">
         <v>140</v>
       </c>
-      <c r="J39" s="39">
+      <c r="J38" s="39">
         <f t="shared" si="2"/>
         <v>640.09120000000007</v>
       </c>
-      <c r="K39" s="39">
+      <c r="K38" s="39">
         <f t="shared" si="3"/>
         <v>1920.2736000000002</v>
       </c>
-      <c r="L39" s="35" t="s">
+      <c r="L38" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="M39" s="35">
+      <c r="M38" s="35">
         <v>62762</v>
       </c>
-      <c r="N39" s="39">
+      <c r="N38" s="39">
         <v>477.68</v>
       </c>
-      <c r="O39" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="P39" s="38">
+      <c r="O38" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="P38" s="38">
         <v>2.68</v>
       </c>
-      <c r="Q39" s="38">
+      <c r="Q38" s="38">
         <v>0.5</v>
       </c>
-      <c r="R39" s="38">
-        <v>1</v>
-      </c>
-      <c r="S39" s="35"/>
-      <c r="T39" s="35"/>
-      <c r="U39" s="35"/>
-      <c r="V39" s="35" t="s">
+      <c r="R38" s="38">
+        <v>1</v>
+      </c>
+      <c r="S38" s="35"/>
+      <c r="T38" s="35"/>
+      <c r="U38" s="35"/>
+      <c r="V38" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="W39" s="35"/>
+      <c r="W38" s="35"/>
+    </row>
+    <row r="39" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D39" s="4">
+        <v>11</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="G39" s="4">
+        <v>1</v>
+      </c>
+      <c r="H39" s="5">
+        <v>15</v>
+      </c>
+      <c r="I39" s="49" t="s">
+        <v>162</v>
+      </c>
+      <c r="J39" s="19">
+        <f t="shared" si="0"/>
+        <v>345.35160000000002</v>
+      </c>
+      <c r="K39" s="19">
+        <f t="shared" si="1"/>
+        <v>5180.2740000000003</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="M39" s="4">
+        <v>3397420</v>
+      </c>
+      <c r="N39" s="19">
+        <v>168.3</v>
+      </c>
+      <c r="O39" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="P39" s="6">
+        <v>3.42</v>
+      </c>
+      <c r="Q39" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="R39" s="6">
+        <v>1</v>
+      </c>
+      <c r="S39" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="T39" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="U39" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="V39" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="40" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
@@ -3863,30 +3884,30 @@
         <v>170</v>
       </c>
       <c r="G40" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H40" s="5">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I40" s="49" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J40" s="19">
         <f t="shared" si="0"/>
-        <v>345.35160000000002</v>
+        <v>215.84987999999998</v>
       </c>
       <c r="K40" s="19">
         <f t="shared" si="1"/>
-        <v>5180.2740000000003</v>
+        <v>2590.1985599999998</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="M40" s="4">
-        <v>3397420</v>
+        <v>3397410</v>
       </c>
       <c r="N40" s="19">
-        <v>168.3</v>
+        <v>105.19</v>
       </c>
       <c r="O40" s="7" t="s">
         <v>2</v>
@@ -3900,20 +3921,11 @@
       <c r="R40" s="6">
         <v>1</v>
       </c>
-      <c r="S40" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="T40" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="U40" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="V40" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" ht="60.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="4" t="s">
         <v>169</v>
       </c>
@@ -3929,111 +3941,126 @@
       <c r="F41" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="G41" s="4">
-        <v>2</v>
-      </c>
-      <c r="H41" s="5">
-        <v>12</v>
-      </c>
-      <c r="I41" s="49" t="s">
-        <v>163</v>
-      </c>
-      <c r="J41" s="19">
-        <f t="shared" si="0"/>
-        <v>215.84987999999998</v>
-      </c>
-      <c r="K41" s="19">
-        <f t="shared" si="1"/>
-        <v>2590.1985599999998</v>
-      </c>
-      <c r="L41" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="M41" s="4">
-        <v>3397410</v>
-      </c>
-      <c r="N41" s="19">
-        <v>105.19</v>
-      </c>
-      <c r="O41" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="P41" s="6">
-        <v>3.42</v>
-      </c>
-      <c r="Q41" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="R41" s="6">
-        <v>1</v>
-      </c>
-      <c r="V41" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="42" spans="1:23" ht="60.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="D42" s="4">
-        <v>11</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="G42" s="35">
+      <c r="G41" s="35">
         <v>3</v>
       </c>
-      <c r="H42" s="36">
+      <c r="H41" s="36">
         <v>10</v>
       </c>
-      <c r="I42" s="50" t="s">
+      <c r="I41" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="J42" s="39">
+      <c r="J41" s="39">
         <f t="shared" si="0"/>
         <v>251.45208000000002</v>
       </c>
-      <c r="K42" s="39">
+      <c r="K41" s="39">
         <f t="shared" si="1"/>
         <v>2514.5208000000002</v>
       </c>
-      <c r="L42" s="35" t="s">
+      <c r="L41" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="M42" s="35">
+      <c r="M41" s="35">
         <v>3397415</v>
       </c>
-      <c r="N42" s="39">
+      <c r="N41" s="39">
         <v>122.54</v>
       </c>
-      <c r="O42" s="40" t="s">
+      <c r="O41" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="P42" s="38">
+      <c r="P41" s="38">
         <v>3.42</v>
       </c>
-      <c r="Q42" s="38">
+      <c r="Q41" s="38">
         <v>0.6</v>
       </c>
-      <c r="R42" s="38">
-        <v>1</v>
-      </c>
-      <c r="S42" s="35"/>
-      <c r="T42" s="35"/>
-      <c r="U42" s="35"/>
-      <c r="V42" s="35" t="s">
+      <c r="R41" s="38">
+        <v>1</v>
+      </c>
+      <c r="S41" s="35"/>
+      <c r="T41" s="35"/>
+      <c r="U41" s="35"/>
+      <c r="V41" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="W42" s="35"/>
-    </row>
-    <row r="43" spans="1:23" ht="72" x14ac:dyDescent="0.25">
+      <c r="W41" s="35"/>
+    </row>
+    <row r="42" spans="1:23" ht="72" x14ac:dyDescent="0.25">
+      <c r="A42" s="75">
+        <v>45352</v>
+      </c>
+      <c r="B42" s="59" t="s">
+        <v>161</v>
+      </c>
+      <c r="C42" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="D42" s="59">
+        <v>12</v>
+      </c>
+      <c r="E42" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="F42" s="59" t="s">
+        <v>176</v>
+      </c>
+      <c r="G42" s="4">
+        <v>1</v>
+      </c>
+      <c r="H42" s="5">
+        <v>1</v>
+      </c>
+      <c r="I42" s="49" t="s">
+        <v>171</v>
+      </c>
+      <c r="J42" s="19">
+        <f>N42*P42*Q42*R42*W42</f>
+        <v>4099.8339839999999</v>
+      </c>
+      <c r="K42" s="19">
+        <f t="shared" si="1"/>
+        <v>4099.8339839999999</v>
+      </c>
+      <c r="L42" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="M42" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="N42" s="19">
+        <v>2683.84</v>
+      </c>
+      <c r="O42" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P42" s="6">
+        <v>2.68</v>
+      </c>
+      <c r="Q42" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="R42" s="6">
+        <v>1</v>
+      </c>
+      <c r="S42" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="T42" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="U42" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="V42" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="W42" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="75">
         <v>45352</v>
       </c>
@@ -4052,109 +4079,91 @@
       <c r="F43" s="59" t="s">
         <v>176</v>
       </c>
-      <c r="G43" s="4">
-        <v>1</v>
-      </c>
-      <c r="H43" s="5">
-        <v>1</v>
-      </c>
-      <c r="I43" s="49" t="s">
-        <v>171</v>
-      </c>
-      <c r="J43" s="19">
-        <f>N43*P43*Q43*R43*W43</f>
-        <v>4099.8339839999999</v>
-      </c>
-      <c r="K43" s="19">
-        <f t="shared" si="1"/>
-        <v>4099.8339839999999</v>
-      </c>
-      <c r="L43" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="M43" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="N43" s="19">
-        <v>2683.84</v>
-      </c>
-      <c r="O43" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="P43" s="6">
-        <v>2.68</v>
-      </c>
-      <c r="Q43" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="R43" s="6">
-        <v>1</v>
-      </c>
-      <c r="S43" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="T43" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="U43" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="V43" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="W43" s="4">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="75">
-        <v>45352</v>
-      </c>
-      <c r="B44" s="59" t="s">
-        <v>161</v>
-      </c>
-      <c r="C44" s="59" t="s">
-        <v>160</v>
-      </c>
-      <c r="D44" s="59">
-        <v>12</v>
-      </c>
-      <c r="E44" s="59" t="s">
-        <v>28</v>
-      </c>
-      <c r="F44" s="59" t="s">
-        <v>176</v>
-      </c>
-      <c r="G44" s="35">
+      <c r="G43" s="35">
         <v>2</v>
       </c>
-      <c r="H44" s="36">
-        <v>1</v>
-      </c>
-      <c r="I44" s="50" t="s">
+      <c r="H43" s="36">
+        <v>1</v>
+      </c>
+      <c r="I43" s="50" t="s">
         <v>174</v>
       </c>
-      <c r="J44" s="39">
+      <c r="J43" s="39">
         <v>1400</v>
       </c>
-      <c r="K44" s="39">
+      <c r="K43" s="39">
         <f t="shared" si="1"/>
         <v>1400</v>
       </c>
-      <c r="L44" s="35" t="s">
+      <c r="L43" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="M44" s="35"/>
-      <c r="N44" s="39"/>
-      <c r="O44" s="40"/>
-      <c r="P44" s="38"/>
-      <c r="Q44" s="38"/>
-      <c r="R44" s="38"/>
-      <c r="S44" s="35"/>
-      <c r="T44" s="35"/>
-      <c r="U44" s="35"/>
-      <c r="V44" s="35"/>
-      <c r="W44" s="35"/>
+      <c r="M43" s="35"/>
+      <c r="N43" s="39"/>
+      <c r="O43" s="40"/>
+      <c r="P43" s="38"/>
+      <c r="Q43" s="38"/>
+      <c r="R43" s="38"/>
+      <c r="S43" s="35"/>
+      <c r="T43" s="35"/>
+      <c r="U43" s="35"/>
+      <c r="V43" s="35"/>
+      <c r="W43" s="35"/>
+    </row>
+    <row r="44" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>45352</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D44" s="4">
+        <v>13</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G44" s="4">
+        <v>1</v>
+      </c>
+      <c r="H44" s="5">
+        <v>4</v>
+      </c>
+      <c r="I44" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="J44" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K44" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L44" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="M44" s="4">
+        <v>66677</v>
+      </c>
+      <c r="N44" s="19">
+        <v>482.6</v>
+      </c>
+      <c r="P44" s="6">
+        <v>2.68</v>
+      </c>
+      <c r="R44" s="6">
+        <v>1</v>
+      </c>
+      <c r="V44" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="45" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
@@ -4176,13 +4185,13 @@
         <v>188</v>
       </c>
       <c r="G45" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H45" s="5">
         <v>4</v>
       </c>
       <c r="I45" s="49" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="J45" s="19">
         <f t="shared" si="0"/>
@@ -4192,14 +4201,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L45" s="4" t="s">
-        <v>130</v>
-      </c>
       <c r="M45" s="4">
-        <v>66677</v>
+        <v>60312</v>
       </c>
       <c r="N45" s="19">
-        <v>482.6</v>
+        <v>70.260000000000005</v>
       </c>
       <c r="P45" s="6">
         <v>2.68</v>
@@ -4222,7 +4228,7 @@
         <v>187</v>
       </c>
       <c r="D46" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>29</v>
@@ -4231,13 +4237,13 @@
         <v>188</v>
       </c>
       <c r="G46" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H46" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I46" s="49" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J46" s="19">
         <f t="shared" si="0"/>
@@ -4247,20 +4253,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M46" s="4">
-        <v>60312</v>
-      </c>
-      <c r="N46" s="19">
-        <v>70.260000000000005</v>
-      </c>
       <c r="P46" s="6">
-        <v>2.68</v>
+        <v>3.42</v>
       </c>
       <c r="R46" s="6">
         <v>1</v>
       </c>
       <c r="V46" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:23" ht="60" x14ac:dyDescent="0.25">
@@ -4283,13 +4283,13 @@
         <v>188</v>
       </c>
       <c r="G47" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H47" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I47" s="49" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J47" s="19">
         <f t="shared" si="0"/>
@@ -4299,17 +4299,20 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="M47" s="4">
+        <v>3397420</v>
+      </c>
+      <c r="N47" s="19">
+        <v>168.3</v>
+      </c>
       <c r="P47" s="6">
         <v>3.42</v>
       </c>
       <c r="R47" s="6">
         <v>1</v>
       </c>
-      <c r="V47" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:23" ht="48" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>45352</v>
       </c>
@@ -4329,13 +4332,13 @@
         <v>188</v>
       </c>
       <c r="G48" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H48" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I48" s="49" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="J48" s="19">
         <f t="shared" si="0"/>
@@ -4346,19 +4349,19 @@
         <v>0</v>
       </c>
       <c r="M48" s="4">
-        <v>3397420</v>
+        <v>224091</v>
       </c>
       <c r="N48" s="19">
-        <v>168.3</v>
+        <v>228.05</v>
       </c>
       <c r="P48" s="6">
-        <v>3.42</v>
+        <v>2.68</v>
       </c>
       <c r="R48" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:23" ht="48" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>45352</v>
       </c>
@@ -4378,13 +4381,13 @@
         <v>188</v>
       </c>
       <c r="G49" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H49" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I49" s="49" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="J49" s="19">
         <f t="shared" si="0"/>
@@ -4395,10 +4398,10 @@
         <v>0</v>
       </c>
       <c r="M49" s="4">
-        <v>224091</v>
+        <v>66673</v>
       </c>
       <c r="N49" s="19">
-        <v>228.05</v>
+        <v>482.6</v>
       </c>
       <c r="P49" s="6">
         <v>2.68</v>
@@ -4407,7 +4410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:23" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>45352</v>
       </c>
@@ -4427,13 +4430,13 @@
         <v>188</v>
       </c>
       <c r="G50" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H50" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I50" s="49" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="J50" s="19">
         <f t="shared" si="0"/>
@@ -4444,10 +4447,10 @@
         <v>0</v>
       </c>
       <c r="M50" s="4">
-        <v>66673</v>
+        <v>60311</v>
       </c>
       <c r="N50" s="19">
-        <v>482.6</v>
+        <v>57.23</v>
       </c>
       <c r="P50" s="6">
         <v>2.68</v>
@@ -4456,7 +4459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:23" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>45352</v>
       </c>
@@ -4476,13 +4479,13 @@
         <v>188</v>
       </c>
       <c r="G51" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H51" s="5">
         <v>5</v>
       </c>
       <c r="I51" s="49" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="J51" s="19">
         <f t="shared" si="0"/>
@@ -4492,20 +4495,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M51" s="4">
-        <v>60311</v>
-      </c>
-      <c r="N51" s="19">
-        <v>57.23</v>
-      </c>
       <c r="P51" s="6">
-        <v>2.68</v>
+        <v>3.42</v>
       </c>
       <c r="R51" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>45352</v>
       </c>
@@ -4525,30 +4522,39 @@
         <v>188</v>
       </c>
       <c r="G52" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H52" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I52" s="49" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="J52" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>251.45208000000002</v>
       </c>
       <c r="K52" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1508.7124800000001</v>
+      </c>
+      <c r="M52" s="4">
+        <v>3397415</v>
+      </c>
+      <c r="N52" s="19">
+        <v>122.54</v>
       </c>
       <c r="P52" s="6">
         <v>3.42</v>
       </c>
+      <c r="Q52" s="6">
+        <v>0.6</v>
+      </c>
       <c r="R52" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:23" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>45352</v>
       </c>
@@ -4567,196 +4573,144 @@
       <c r="F53" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="G53" s="4">
-        <v>9</v>
-      </c>
-      <c r="H53" s="5">
-        <v>6</v>
-      </c>
-      <c r="I53" s="49" t="s">
-        <v>190</v>
-      </c>
-      <c r="J53" s="19">
+      <c r="G53" s="35">
+        <v>10</v>
+      </c>
+      <c r="H53" s="36">
+        <v>3</v>
+      </c>
+      <c r="I53" s="50" t="s">
+        <v>185</v>
+      </c>
+      <c r="J53" s="39">
         <f t="shared" si="0"/>
-        <v>251.45208000000002</v>
-      </c>
-      <c r="K53" s="19">
+        <v>252.36220000000003</v>
+      </c>
+      <c r="K53" s="39">
         <f t="shared" si="1"/>
-        <v>1508.7124800000001</v>
-      </c>
-      <c r="M53" s="4">
-        <v>3397415</v>
-      </c>
-      <c r="N53" s="19">
-        <v>122.54</v>
-      </c>
-      <c r="P53" s="6">
-        <v>3.42</v>
-      </c>
-      <c r="Q53" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="R53" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>757.08660000000009</v>
+      </c>
+      <c r="L53" s="35"/>
+      <c r="M53" s="35">
+        <v>223091</v>
+      </c>
+      <c r="N53" s="39">
+        <v>188.33</v>
+      </c>
+      <c r="O53" s="40"/>
+      <c r="P53" s="38">
+        <v>2.68</v>
+      </c>
+      <c r="Q53" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="R53" s="38">
+        <v>1</v>
+      </c>
+      <c r="S53" s="35"/>
+      <c r="T53" s="35"/>
+      <c r="U53" s="35"/>
+      <c r="V53" s="35"/>
+      <c r="W53" s="35"/>
+    </row>
+    <row r="54" spans="1:23" ht="168" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>45352</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="D54" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="G54" s="35">
-        <v>10</v>
-      </c>
-      <c r="H54" s="36">
-        <v>3</v>
-      </c>
-      <c r="I54" s="50" t="s">
-        <v>185</v>
-      </c>
-      <c r="J54" s="39">
-        <f t="shared" si="0"/>
-        <v>252.36220000000003</v>
-      </c>
-      <c r="K54" s="39">
-        <f t="shared" si="1"/>
-        <v>757.08660000000009</v>
-      </c>
-      <c r="L54" s="35"/>
-      <c r="M54" s="35">
-        <v>223091</v>
-      </c>
-      <c r="N54" s="39">
-        <v>188.33</v>
-      </c>
-      <c r="O54" s="40"/>
-      <c r="P54" s="38">
-        <v>2.68</v>
-      </c>
-      <c r="Q54" s="38">
-        <v>0.5</v>
-      </c>
-      <c r="R54" s="38">
-        <v>1</v>
-      </c>
-      <c r="S54" s="35"/>
-      <c r="T54" s="35"/>
-      <c r="U54" s="35"/>
-      <c r="V54" s="35"/>
-      <c r="W54" s="35"/>
-    </row>
-    <row r="55" spans="1:23" ht="168" x14ac:dyDescent="0.25">
-      <c r="A55" s="3">
-        <v>45352</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D55" s="4">
-        <v>15</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F55" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="G55" s="4">
-        <v>1</v>
-      </c>
-      <c r="H55" s="5">
-        <v>1</v>
-      </c>
-      <c r="I55" s="49" t="s">
+      <c r="G54" s="4">
+        <v>1</v>
+      </c>
+      <c r="H54" s="5">
+        <v>1</v>
+      </c>
+      <c r="I54" s="49" t="s">
         <v>191</v>
       </c>
-      <c r="J55" s="19">
+      <c r="J54" s="19">
         <v>5235.45</v>
       </c>
-      <c r="K55" s="19">
+      <c r="K54" s="19">
         <f t="shared" si="1"/>
         <v>5235.45</v>
       </c>
-      <c r="S55" s="4" t="s">
+      <c r="S54" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="T55" s="4" t="s">
+      <c r="T54" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="U55" s="4" t="s">
+      <c r="U54" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="V55" s="4" t="s">
+      <c r="V54" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:23" ht="48.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="76">
+    <row r="55" spans="1:23" ht="48.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="76">
         <v>45352</v>
       </c>
-      <c r="B56" s="77" t="s">
+      <c r="B55" s="77" t="s">
         <v>194</v>
       </c>
-      <c r="C56" s="77" t="s">
+      <c r="C55" s="77" t="s">
         <v>193</v>
       </c>
-      <c r="D56" s="77">
+      <c r="D55" s="77">
         <v>15</v>
       </c>
-      <c r="E56" s="77" t="s">
+      <c r="E55" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="F56" s="77" t="s">
+      <c r="F55" s="77" t="s">
         <v>195</v>
       </c>
-      <c r="G56" s="35">
+      <c r="G55" s="35">
         <v>2</v>
       </c>
-      <c r="H56" s="36">
-        <v>1</v>
-      </c>
-      <c r="I56" s="50" t="s">
+      <c r="H55" s="36">
+        <v>1</v>
+      </c>
+      <c r="I55" s="50" t="s">
         <v>192</v>
       </c>
-      <c r="J56" s="39">
+      <c r="J55" s="39">
         <v>13484.1</v>
       </c>
-      <c r="K56" s="39">
+      <c r="K55" s="39">
         <f t="shared" si="1"/>
         <v>13484.1</v>
       </c>
-      <c r="L56" s="35"/>
-      <c r="M56" s="35"/>
-      <c r="N56" s="39"/>
-      <c r="O56" s="40"/>
-      <c r="P56" s="38"/>
-      <c r="Q56" s="38"/>
-      <c r="R56" s="38"/>
-      <c r="S56" s="35"/>
-      <c r="T56" s="35"/>
-      <c r="U56" s="35"/>
-      <c r="V56" s="35"/>
-      <c r="W56" s="35"/>
-    </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I66" s="78"/>
+      <c r="L55" s="35"/>
+      <c r="M55" s="35"/>
+      <c r="N55" s="39"/>
+      <c r="O55" s="40"/>
+      <c r="P55" s="38"/>
+      <c r="Q55" s="38"/>
+      <c r="R55" s="38"/>
+      <c r="S55" s="35"/>
+      <c r="T55" s="35"/>
+      <c r="U55" s="35"/>
+      <c r="V55" s="35"/>
+      <c r="W55" s="35"/>
+    </row>
+    <row r="65" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I65" s="78"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4764,23 +4718,23 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C3489894-BA8C-4847-B1CC-6ED46AD2B826}">
+          <x14:formula1>
+            <xm:f>Hoja3!$F$2:$F$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>V1 V56:V1048576 V3:V28</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F57BF4DB-265C-449B-B766-F25913BB2489}">
+          <x14:formula1>
+            <xm:f>Hoja3!$F$2:$F$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>V2 V29:V55</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F7DD91D3-8581-4234-BFA7-90C564303799}">
           <x14:formula1>
             <xm:f>Hoja3!$H$2:$H$7</xm:f>
           </x14:formula1>
           <xm:sqref>E1:E1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C3489894-BA8C-4847-B1CC-6ED46AD2B826}">
-          <x14:formula1>
-            <xm:f>Hoja3!$F$2:$F$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>V1 V3:V29 V57:V1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F57BF4DB-265C-449B-B766-F25913BB2489}">
-          <x14:formula1>
-            <xm:f>Hoja3!$F$2:$F$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>V2 V30:V56</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F98475A1-8BD8-4054-9CB4-A8337C0A78DA}">
           <x14:formula1>
@@ -4856,7 +4810,7 @@
         <v>65</v>
       </c>
       <c r="B6" s="23" t="str">
-        <f>Hoja1!B55</f>
+        <f>Hoja1!B54</f>
         <v xml:space="preserve">ALIMENTOS POLAR COMERCIAL </v>
       </c>
       <c r="C6" s="24"/>
@@ -4864,7 +4818,7 @@
         <v>68</v>
       </c>
       <c r="E6" s="32" t="str">
-        <f>Hoja1!F55</f>
+        <f>Hoja1!F54</f>
         <v>TF-CN-01-03-001-BQTO</v>
       </c>
       <c r="F6" s="30"/>
@@ -4874,7 +4828,7 @@
         <v>66</v>
       </c>
       <c r="B7" s="23" t="str">
-        <f>Hoja1!C55</f>
+        <f>Hoja1!C54</f>
         <v>SHEYLA MARIA REYES ALVAREZ</v>
       </c>
       <c r="C7" s="23"/>
@@ -4882,7 +4836,7 @@
         <v>67</v>
       </c>
       <c r="E7" s="80">
-        <f>Hoja1!D55</f>
+        <f>Hoja1!D54</f>
         <v>15</v>
       </c>
       <c r="F7" s="81"/>
@@ -4944,7 +4898,7 @@
         <v>5235.45</v>
       </c>
       <c r="F13" s="72" t="str">
-        <f>Hoja1!V43</f>
+        <f>Hoja1!V42</f>
         <v>04 - 06 semanas</v>
       </c>
     </row>

</xml_diff>